<commit_message>
2 commit del dia
</commit_message>
<xml_diff>
--- a/CajaInternet.xlsx
+++ b/CajaInternet.xlsx
@@ -177,6 +177,15 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -184,15 +193,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -478,7 +478,7 @@
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,50 +489,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16"/>
-      <c r="G1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16"/>
-      <c r="M1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="16"/>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
+      <c r="G1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="13"/>
+      <c r="M1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="13"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="14">
         <v>43254</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="G2" s="11">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="G2" s="14">
         <v>43261</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="13"/>
-      <c r="M2" s="11">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
+      <c r="M2" s="14">
         <v>43268</v>
       </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="13"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="16"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -626,10 +626,12 @@
         <f t="shared" ref="O4:O13" si="1">SUM(M4*N4)</f>
         <v>0.25</v>
       </c>
-      <c r="P4" s="1"/>
+      <c r="P4" s="1">
+        <v>5</v>
+      </c>
       <c r="Q4" s="2">
         <f>SUM(M4*P4)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -677,10 +679,12 @@
         <f t="shared" si="1"/>
         <v>1.9000000000000001</v>
       </c>
-      <c r="P5" s="1"/>
+      <c r="P5" s="1">
+        <v>19</v>
+      </c>
       <c r="Q5" s="2">
         <f>SUM(M5*P5)</f>
-        <v>0</v>
+        <v>1.9000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -728,10 +732,12 @@
         <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1">
+        <v>15</v>
+      </c>
       <c r="Q6" s="2">
         <f t="shared" ref="Q6:Q13" si="5">SUM(M6*P6)</f>
-        <v>0</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -779,10 +785,12 @@
         <f t="shared" si="1"/>
         <v>14.5</v>
       </c>
-      <c r="P7" s="1"/>
+      <c r="P7" s="1">
+        <v>29</v>
+      </c>
       <c r="Q7" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -830,10 +838,12 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1">
+        <v>13</v>
+      </c>
       <c r="Q8" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -881,10 +891,12 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="P9" s="1"/>
+      <c r="P9" s="1">
+        <v>9</v>
+      </c>
       <c r="Q9" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -932,10 +944,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P10" s="1"/>
+      <c r="P10" s="1">
+        <v>4</v>
+      </c>
       <c r="Q10" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -983,7 +997,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P11" s="1"/>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
       <c r="Q11" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -1034,10 +1050,12 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="P12" s="1"/>
+      <c r="P12" s="1">
+        <v>2</v>
+      </c>
       <c r="Q12" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1085,7 +1103,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P13" s="1"/>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
       <c r="Q13" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -1129,31 +1149,31 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="2">
         <f>SUM(Q4:Q13)</f>
-        <v>0</v>
+        <v>218.4</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-      <c r="G17" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="16"/>
-      <c r="M17" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="16"/>
+      <c r="A17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
+      <c r="G17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="13"/>
+      <c r="M17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="13"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
@@ -1671,44 +1691,44 @@
       </c>
     </row>
     <row r="33" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16"/>
-      <c r="G33" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="16"/>
-      <c r="M33" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="16"/>
+      <c r="A33" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13"/>
+      <c r="G33" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="13"/>
+      <c r="M33" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="13"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="13"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="13"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="16"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="16"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="16"/>
     </row>
     <row r="35" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
@@ -2210,6 +2230,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="M34:Q34"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="M33:Q33"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="G17:K17"/>
     <mergeCell ref="M17:Q17"/>
@@ -2219,12 +2245,6 @@
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="G2:K2"/>
-    <mergeCell ref="M34:Q34"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="M33:Q33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>